<commit_message>
search for test no need to install sqllite on Dockerfile
</commit_message>
<xml_diff>
--- a/Datentreiber.xlsx
+++ b/Datentreiber.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnaas\IdeaProjects\VakanzenGrabber\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aseverin\IdeaProjects\VakanzenGrabber-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BAE7A0-4715-4E5D-BB06-30C544E9D044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87FDCB4-E2AC-4FDD-B28A-10D548C3D228}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testdaten" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <t>Suchbegriff</t>
   </si>
   <si>
-    <t>Testanalyst</t>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -872,20 +872,20 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -904,7 +904,7 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -916,7 +916,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -928,7 +928,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>